<commit_message>
update info and added new house TAMASHA
</commit_message>
<xml_diff>
--- a/BAIMURA.xlsx
+++ b/BAIMURA.xlsx
@@ -2,22 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -37,14 +37,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0000FF00"/>
-        <bgColor rgb="0000FF00"/>
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00FF0000"/>
+        <fgColor rgb="0000FF00"/>
+        <bgColor rgb="0000FF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -60,14 +60,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -430,13 +433,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:O72"/>
+  <dimension ref="A3:O93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="10.42578125" bestFit="1" customWidth="1" style="3" min="7" max="7"/>
+    <col width="12.5703125" bestFit="1" customWidth="1" style="3" min="9" max="9"/>
+    <col width="10.42578125" bestFit="1" customWidth="1" style="3" min="10" max="10"/>
+    <col width="10.42578125" bestFit="1" customWidth="1" style="3" min="13" max="13"/>
+  </cols>
   <sheetData>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -506,7 +515,15 @@
           <t xml:space="preserve">5 </t>
         </is>
       </c>
-      <c r="G4" s="1" t="n"/>
+      <c r="G4" s="2" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H4" t="n">
+        <v>509000</v>
+      </c>
+      <c r="I4" t="n">
+        <v>18894080</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -534,7 +551,7 @@
           <t xml:space="preserve">3 </t>
         </is>
       </c>
-      <c r="G5" s="1" t="n"/>
+      <c r="G5" s="2" t="n"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -562,33 +579,25 @@
           <t xml:space="preserve">5 </t>
         </is>
       </c>
-      <c r="G6" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="H6" s="2" t="n">
+      <c r="G6" s="2" t="n">
+        <v>45635</v>
+      </c>
+      <c r="H6" t="n">
         <v>505000</v>
       </c>
       <c r="I6" t="n">
         <v>18755700</v>
       </c>
-      <c r="J6" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="K6" t="n">
-        <v>505000</v>
+      <c r="J6" s="2" t="n">
+        <v>45648</v>
+      </c>
+      <c r="K6" s="4" t="n">
+        <v>509000</v>
       </c>
       <c r="L6" t="n">
-        <v>18755700</v>
-      </c>
-      <c r="M6" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N6" t="n">
-        <v>505000</v>
-      </c>
-      <c r="O6" t="n">
-        <v>18755700</v>
-      </c>
+        <v>18904260</v>
+      </c>
+      <c r="M6" s="2" t="n"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -616,33 +625,25 @@
           <t xml:space="preserve">7 </t>
         </is>
       </c>
-      <c r="G7" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="H7" s="2" t="n">
+      <c r="G7" s="2" t="n">
+        <v>45635</v>
+      </c>
+      <c r="H7" t="n">
         <v>504000</v>
       </c>
       <c r="I7" t="n">
         <v>18879840</v>
       </c>
-      <c r="J7" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="K7" t="n">
-        <v>504000</v>
+      <c r="J7" s="2" t="n">
+        <v>45648</v>
+      </c>
+      <c r="K7" s="4" t="n">
+        <v>509000</v>
       </c>
       <c r="L7" t="n">
-        <v>18879840</v>
-      </c>
-      <c r="M7" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N7" t="n">
-        <v>504000</v>
-      </c>
-      <c r="O7" t="n">
-        <v>18879840</v>
-      </c>
+        <v>19067140</v>
+      </c>
+      <c r="M7" s="2" t="n"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -670,33 +671,25 @@
           <t xml:space="preserve">5 </t>
         </is>
       </c>
-      <c r="G8" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="H8" s="3" t="n">
+      <c r="G8" s="2" t="n">
+        <v>45635</v>
+      </c>
+      <c r="H8" t="n">
         <v>497000</v>
       </c>
       <c r="I8" t="n">
         <v>19542040</v>
       </c>
-      <c r="J8" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="K8" t="n">
-        <v>497000</v>
+      <c r="J8" s="2" t="n">
+        <v>45648</v>
+      </c>
+      <c r="K8" s="4" t="n">
+        <v>499000</v>
       </c>
       <c r="L8" t="n">
-        <v>19542040</v>
-      </c>
-      <c r="M8" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N8" t="n">
-        <v>497000</v>
-      </c>
-      <c r="O8" t="n">
-        <v>19542040</v>
-      </c>
+        <v>19620680</v>
+      </c>
+      <c r="M8" s="2" t="n"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -724,33 +717,25 @@
           <t xml:space="preserve">3 </t>
         </is>
       </c>
-      <c r="G9" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="H9" s="3" t="n">
+      <c r="G9" s="2" t="n">
+        <v>45635</v>
+      </c>
+      <c r="H9" t="n">
         <v>509000</v>
       </c>
       <c r="I9" t="n">
         <v>19825550</v>
       </c>
-      <c r="J9" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="K9" s="2" t="n">
-        <v>503000</v>
+      <c r="J9" s="2" t="n">
+        <v>45648</v>
+      </c>
+      <c r="K9" s="5" t="n">
+        <v>504000</v>
       </c>
       <c r="L9" t="n">
-        <v>19591850</v>
-      </c>
-      <c r="M9" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N9" t="n">
-        <v>503000</v>
-      </c>
-      <c r="O9" t="n">
-        <v>19591850</v>
-      </c>
+        <v>19630800</v>
+      </c>
+      <c r="M9" s="2" t="n"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -778,33 +763,25 @@
           <t xml:space="preserve">3 </t>
         </is>
       </c>
-      <c r="G10" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="H10" s="3" t="n">
+      <c r="G10" s="2" t="n">
+        <v>45635</v>
+      </c>
+      <c r="H10" t="n">
         <v>508000</v>
       </c>
       <c r="I10" t="n">
         <v>19939000</v>
       </c>
-      <c r="J10" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="K10" t="n">
-        <v>508000</v>
+      <c r="J10" s="2" t="n">
+        <v>45648</v>
+      </c>
+      <c r="K10" s="5" t="n">
+        <v>504000</v>
       </c>
       <c r="L10" t="n">
-        <v>19939000</v>
-      </c>
-      <c r="M10" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N10" t="n">
-        <v>508000</v>
-      </c>
-      <c r="O10" t="n">
-        <v>19939000</v>
-      </c>
+        <v>19782000</v>
+      </c>
+      <c r="M10" s="2" t="n"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -832,7 +809,7 @@
           <t xml:space="preserve">3 </t>
         </is>
       </c>
-      <c r="G11" s="1" t="n">
+      <c r="G11" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H11" t="n">
@@ -841,8 +818,8 @@
       <c r="I11" t="n">
         <v>20215050</v>
       </c>
-      <c r="J11" s="1" t="n">
-        <v>45635</v>
+      <c r="J11" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K11" t="n">
         <v>519000</v>
@@ -850,15 +827,7 @@
       <c r="L11" t="n">
         <v>20215050</v>
       </c>
-      <c r="M11" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N11" t="n">
-        <v>519000</v>
-      </c>
-      <c r="O11" t="n">
-        <v>20215050</v>
-      </c>
+      <c r="M11" s="2" t="n"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -886,33 +855,17 @@
           <t xml:space="preserve">7 </t>
         </is>
       </c>
-      <c r="G12" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="H12" s="2" t="n">
+      <c r="G12" s="2" t="n">
+        <v>45635</v>
+      </c>
+      <c r="H12" t="n">
         <v>516000</v>
       </c>
       <c r="I12" t="n">
         <v>20366520</v>
       </c>
-      <c r="J12" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="K12" s="3" t="n">
-        <v>532000</v>
-      </c>
-      <c r="L12" t="n">
-        <v>20998040</v>
-      </c>
-      <c r="M12" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N12" t="n">
-        <v>532000</v>
-      </c>
-      <c r="O12" t="n">
-        <v>20998040</v>
-      </c>
+      <c r="J12" s="2" t="n"/>
+      <c r="M12" s="2" t="n"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -940,10 +893,10 @@
           <t xml:space="preserve">7 </t>
         </is>
       </c>
-      <c r="G13" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="H13" s="3" t="n">
+      <c r="G13" s="2" t="n">
+        <v>45635</v>
+      </c>
+      <c r="H13" t="n">
         <v>518000</v>
       </c>
       <c r="I13" t="n">
@@ -976,7 +929,15 @@
           <t xml:space="preserve">1 </t>
         </is>
       </c>
-      <c r="G14" s="1" t="n"/>
+      <c r="G14" s="2" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H14" t="n">
+        <v>519000</v>
+      </c>
+      <c r="I14" t="n">
+        <v>20292900</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1004,15 +965,24 @@
           <t xml:space="preserve">1 </t>
         </is>
       </c>
-      <c r="G15" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="H15" s="2" t="n">
+      <c r="G15" s="2" t="n">
+        <v>45635</v>
+      </c>
+      <c r="H15" t="n">
         <v>497000</v>
       </c>
       <c r="I15" t="n">
         <v>20237840</v>
       </c>
+      <c r="J15" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="K15" s="4" t="n">
+        <v>499000</v>
+      </c>
+      <c r="L15" t="n">
+        <v>20319280</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1040,15 +1010,24 @@
           <t xml:space="preserve">3 </t>
         </is>
       </c>
-      <c r="G16" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="H16" s="2" t="n">
+      <c r="G16" s="2" t="n">
+        <v>45635</v>
+      </c>
+      <c r="H16" t="n">
         <v>466000</v>
       </c>
       <c r="I16" t="n">
         <v>20257020</v>
       </c>
+      <c r="J16" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="K16" s="4" t="n">
+        <v>469000</v>
+      </c>
+      <c r="L16" t="n">
+        <v>20387430</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1076,15 +1055,24 @@
           <t xml:space="preserve">1 </t>
         </is>
       </c>
-      <c r="G17" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="H17" s="3" t="n">
+      <c r="G17" s="2" t="n">
+        <v>45635</v>
+      </c>
+      <c r="H17" t="n">
         <v>519000</v>
       </c>
       <c r="I17" t="n">
         <v>20770380</v>
       </c>
+      <c r="J17" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="K17" s="5" t="n">
+        <v>514000</v>
+      </c>
+      <c r="L17" t="n">
+        <v>20570280</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1112,7 +1100,7 @@
           <t xml:space="preserve">1 </t>
         </is>
       </c>
-      <c r="G18" s="1" t="n">
+      <c r="G18" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H18" t="n">
@@ -1121,8 +1109,8 @@
       <c r="I18" t="n">
         <v>20588740</v>
       </c>
-      <c r="J18" s="1" t="n">
-        <v>45635</v>
+      <c r="J18" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K18" t="n">
         <v>499000</v>
@@ -1130,15 +1118,7 @@
       <c r="L18" t="n">
         <v>20588740</v>
       </c>
-      <c r="M18" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N18" t="n">
-        <v>499000</v>
-      </c>
-      <c r="O18" t="n">
-        <v>20588740</v>
-      </c>
+      <c r="M18" s="2" t="n"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1166,33 +1146,25 @@
           <t xml:space="preserve">1 </t>
         </is>
       </c>
-      <c r="G19" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="H19" s="3" t="n">
+      <c r="G19" s="2" t="n">
+        <v>45635</v>
+      </c>
+      <c r="H19" t="n">
         <v>509000</v>
       </c>
       <c r="I19" t="n">
         <v>21001340</v>
       </c>
-      <c r="J19" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="K19" t="n">
-        <v>509000</v>
+      <c r="J19" s="2" t="n">
+        <v>45648</v>
+      </c>
+      <c r="K19" s="5" t="n">
+        <v>504000</v>
       </c>
       <c r="L19" t="n">
-        <v>21001340</v>
-      </c>
-      <c r="M19" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N19" t="n">
-        <v>509000</v>
-      </c>
-      <c r="O19" t="n">
-        <v>21001340</v>
-      </c>
+        <v>20795040</v>
+      </c>
+      <c r="M19" s="2" t="n"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1220,7 +1192,7 @@
           <t xml:space="preserve">1 </t>
         </is>
       </c>
-      <c r="G20" s="1" t="n">
+      <c r="G20" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H20" t="n">
@@ -1229,6 +1201,15 @@
       <c r="I20" t="n">
         <v>20868400</v>
       </c>
+      <c r="J20" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="K20" t="n">
+        <v>514000</v>
+      </c>
+      <c r="L20" t="n">
+        <v>20868400</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1256,7 +1237,7 @@
           <t xml:space="preserve">1 </t>
         </is>
       </c>
-      <c r="G21" s="1" t="n">
+      <c r="G21" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H21" t="n">
@@ -1265,8 +1246,8 @@
       <c r="I21" t="n">
         <v>20892840</v>
       </c>
-      <c r="J21" s="1" t="n">
-        <v>45635</v>
+      <c r="J21" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K21" t="n">
         <v>516000</v>
@@ -1274,15 +1255,7 @@
       <c r="L21" t="n">
         <v>20892840</v>
       </c>
-      <c r="M21" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N21" t="n">
-        <v>516000</v>
-      </c>
-      <c r="O21" t="n">
-        <v>20892840</v>
-      </c>
+      <c r="M21" s="2" t="n"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1310,7 +1283,7 @@
           <t xml:space="preserve">1 </t>
         </is>
       </c>
-      <c r="G22" s="1" t="n">
+      <c r="G22" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H22" t="n">
@@ -1319,8 +1292,8 @@
       <c r="I22" t="n">
         <v>20892840</v>
       </c>
-      <c r="J22" s="1" t="n">
-        <v>45635</v>
+      <c r="J22" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K22" t="n">
         <v>516000</v>
@@ -1328,15 +1301,7 @@
       <c r="L22" t="n">
         <v>20892840</v>
       </c>
-      <c r="M22" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N22" t="n">
-        <v>516000</v>
-      </c>
-      <c r="O22" t="n">
-        <v>20892840</v>
-      </c>
+      <c r="M22" s="2" t="n"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1364,7 +1329,7 @@
           <t xml:space="preserve">1 </t>
         </is>
       </c>
-      <c r="G23" s="1" t="n">
+      <c r="G23" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H23" t="n">
@@ -1373,8 +1338,8 @@
       <c r="I23" t="n">
         <v>20930080</v>
       </c>
-      <c r="J23" s="1" t="n">
-        <v>45635</v>
+      <c r="J23" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K23" t="n">
         <v>514000</v>
@@ -1382,15 +1347,7 @@
       <c r="L23" t="n">
         <v>20930080</v>
       </c>
-      <c r="M23" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N23" t="n">
-        <v>514000</v>
-      </c>
-      <c r="O23" t="n">
-        <v>20930080</v>
-      </c>
+      <c r="M23" s="2" t="n"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1418,7 +1375,7 @@
           <t xml:space="preserve">3 </t>
         </is>
       </c>
-      <c r="G24" s="1" t="n">
+      <c r="G24" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H24" t="n">
@@ -1427,8 +1384,8 @@
       <c r="I24" t="n">
         <v>21039480</v>
       </c>
-      <c r="J24" s="1" t="n">
-        <v>45635</v>
+      <c r="J24" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K24" t="n">
         <v>484000</v>
@@ -1436,15 +1393,7 @@
       <c r="L24" t="n">
         <v>21039480</v>
       </c>
-      <c r="M24" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N24" t="n">
-        <v>484000</v>
-      </c>
-      <c r="O24" t="n">
-        <v>21039480</v>
-      </c>
+      <c r="M24" s="2" t="n"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1472,7 +1421,7 @@
           <t xml:space="preserve">1 </t>
         </is>
       </c>
-      <c r="G25" s="1" t="n">
+      <c r="G25" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H25" t="n">
@@ -1481,8 +1430,8 @@
       <c r="I25" t="n">
         <v>21207640</v>
       </c>
-      <c r="J25" s="1" t="n">
-        <v>45635</v>
+      <c r="J25" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K25" t="n">
         <v>514000</v>
@@ -1490,15 +1439,7 @@
       <c r="L25" t="n">
         <v>21207640</v>
       </c>
-      <c r="M25" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N25" t="n">
-        <v>514000</v>
-      </c>
-      <c r="O25" t="n">
-        <v>21207640</v>
-      </c>
+      <c r="M25" s="2" t="n"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1526,7 +1467,7 @@
           <t xml:space="preserve">3 </t>
         </is>
       </c>
-      <c r="G26" s="1" t="n">
+      <c r="G26" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H26" t="n">
@@ -1535,8 +1476,8 @@
       <c r="I26" t="n">
         <v>21399840</v>
       </c>
-      <c r="J26" s="1" t="n">
-        <v>45635</v>
+      <c r="J26" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K26" t="n">
         <v>504000</v>
@@ -1544,15 +1485,7 @@
       <c r="L26" t="n">
         <v>21399840</v>
       </c>
-      <c r="M26" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N26" t="n">
-        <v>504000</v>
-      </c>
-      <c r="O26" t="n">
-        <v>21399840</v>
-      </c>
+      <c r="M26" s="2" t="n"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1580,7 +1513,7 @@
           <t xml:space="preserve">3 </t>
         </is>
       </c>
-      <c r="G27" s="1" t="n">
+      <c r="G27" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H27" t="n">
@@ -1589,8 +1522,8 @@
       <c r="I27" t="n">
         <v>21399840</v>
       </c>
-      <c r="J27" s="1" t="n">
-        <v>45635</v>
+      <c r="J27" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K27" t="n">
         <v>504000</v>
@@ -1598,15 +1531,7 @@
       <c r="L27" t="n">
         <v>21399840</v>
       </c>
-      <c r="M27" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N27" t="n">
-        <v>504000</v>
-      </c>
-      <c r="O27" t="n">
-        <v>21399840</v>
-      </c>
+      <c r="M27" s="2" t="n"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1634,7 +1559,7 @@
           <t xml:space="preserve">1 </t>
         </is>
       </c>
-      <c r="G28" s="1" t="n">
+      <c r="G28" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H28" t="n">
@@ -1643,8 +1568,8 @@
       <c r="I28" t="n">
         <v>21538000</v>
       </c>
-      <c r="J28" s="1" t="n">
-        <v>45635</v>
+      <c r="J28" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K28" t="n">
         <v>484000</v>
@@ -1652,15 +1577,7 @@
       <c r="L28" t="n">
         <v>21538000</v>
       </c>
-      <c r="M28" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N28" t="n">
-        <v>484000</v>
-      </c>
-      <c r="O28" t="n">
-        <v>21538000</v>
-      </c>
+      <c r="M28" s="2" t="n"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1688,7 +1605,7 @@
           <t xml:space="preserve">1 </t>
         </is>
       </c>
-      <c r="G29" s="1" t="n">
+      <c r="G29" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H29" t="n">
@@ -1697,8 +1614,8 @@
       <c r="I29" t="n">
         <v>21538000</v>
       </c>
-      <c r="J29" s="1" t="n">
-        <v>45635</v>
+      <c r="J29" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K29" t="n">
         <v>484000</v>
@@ -1706,15 +1623,7 @@
       <c r="L29" t="n">
         <v>21538000</v>
       </c>
-      <c r="M29" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N29" t="n">
-        <v>484000</v>
-      </c>
-      <c r="O29" t="n">
-        <v>21538000</v>
-      </c>
+      <c r="M29" s="2" t="n"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1742,7 +1651,7 @@
           <t xml:space="preserve">1 </t>
         </is>
       </c>
-      <c r="G30" s="1" t="n">
+      <c r="G30" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H30" t="n">
@@ -1751,8 +1660,8 @@
       <c r="I30" t="n">
         <v>21538000</v>
       </c>
-      <c r="J30" s="1" t="n">
-        <v>45635</v>
+      <c r="J30" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K30" t="n">
         <v>484000</v>
@@ -1760,15 +1669,7 @@
       <c r="L30" t="n">
         <v>21538000</v>
       </c>
-      <c r="M30" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N30" t="n">
-        <v>484000</v>
-      </c>
-      <c r="O30" t="n">
-        <v>21538000</v>
-      </c>
+      <c r="M30" s="2" t="n"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1796,7 +1697,7 @@
           <t xml:space="preserve">1 </t>
         </is>
       </c>
-      <c r="G31" s="1" t="n">
+      <c r="G31" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H31" t="n">
@@ -1805,8 +1706,8 @@
       <c r="I31" t="n">
         <v>21538000</v>
       </c>
-      <c r="J31" s="1" t="n">
-        <v>45635</v>
+      <c r="J31" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K31" t="n">
         <v>484000</v>
@@ -1814,15 +1715,7 @@
       <c r="L31" t="n">
         <v>21538000</v>
       </c>
-      <c r="M31" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N31" t="n">
-        <v>484000</v>
-      </c>
-      <c r="O31" t="n">
-        <v>21538000</v>
-      </c>
+      <c r="M31" s="2" t="n"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1850,7 +1743,7 @@
           <t xml:space="preserve">1 </t>
         </is>
       </c>
-      <c r="G32" s="1" t="n">
+      <c r="G32" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H32" t="n">
@@ -1859,8 +1752,8 @@
       <c r="I32" t="n">
         <v>21663440</v>
       </c>
-      <c r="J32" s="1" t="n">
-        <v>45635</v>
+      <c r="J32" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K32" t="n">
         <v>468500</v>
@@ -1868,15 +1761,7 @@
       <c r="L32" t="n">
         <v>21663440</v>
       </c>
-      <c r="M32" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N32" t="n">
-        <v>468500</v>
-      </c>
-      <c r="O32" t="n">
-        <v>21663440</v>
-      </c>
+      <c r="M32" s="2" t="n"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1904,7 +1789,7 @@
           <t xml:space="preserve">6 </t>
         </is>
       </c>
-      <c r="G33" s="1" t="n">
+      <c r="G33" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H33" t="n">
@@ -1913,8 +1798,8 @@
       <c r="I33" t="n">
         <v>22062740</v>
       </c>
-      <c r="J33" s="1" t="n">
-        <v>45635</v>
+      <c r="J33" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K33" t="n">
         <v>479000</v>
@@ -1922,15 +1807,7 @@
       <c r="L33" t="n">
         <v>22062740</v>
       </c>
-      <c r="M33" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N33" t="n">
-        <v>479000</v>
-      </c>
-      <c r="O33" t="n">
-        <v>22062740</v>
-      </c>
+      <c r="M33" s="2" t="n"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1958,7 +1835,7 @@
           <t xml:space="preserve">6 </t>
         </is>
       </c>
-      <c r="G34" s="1" t="n">
+      <c r="G34" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H34" t="n">
@@ -1967,8 +1844,8 @@
       <c r="I34" t="n">
         <v>22828800</v>
       </c>
-      <c r="J34" s="1" t="n">
-        <v>45635</v>
+      <c r="J34" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K34" t="n">
         <v>435000</v>
@@ -2003,7 +1880,7 @@
           <t xml:space="preserve">2 </t>
         </is>
       </c>
-      <c r="G35" s="1" t="n">
+      <c r="G35" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H35" t="n">
@@ -2012,8 +1889,8 @@
       <c r="I35" t="n">
         <v>24629320</v>
       </c>
-      <c r="J35" s="1" t="n">
-        <v>45635</v>
+      <c r="J35" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K35" t="n">
         <v>437000</v>
@@ -2048,7 +1925,7 @@
           <t xml:space="preserve">2 </t>
         </is>
       </c>
-      <c r="G36" s="1" t="n">
+      <c r="G36" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H36" t="n">
@@ -2057,8 +1934,8 @@
       <c r="I36" t="n">
         <v>27525240</v>
       </c>
-      <c r="J36" s="1" t="n">
-        <v>45635</v>
+      <c r="J36" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K36" t="n">
         <v>471000</v>
@@ -2066,15 +1943,7 @@
       <c r="L36" t="n">
         <v>27525240</v>
       </c>
-      <c r="M36" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N36" s="3" t="n">
-        <v>475000</v>
-      </c>
-      <c r="O36" t="n">
-        <v>27759000</v>
-      </c>
+      <c r="M36" s="2" t="n"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2102,7 +1971,7 @@
           <t xml:space="preserve">2 </t>
         </is>
       </c>
-      <c r="G37" s="1" t="n">
+      <c r="G37" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H37" t="n">
@@ -2111,8 +1980,8 @@
       <c r="I37" t="n">
         <v>27569070</v>
       </c>
-      <c r="J37" s="1" t="n">
-        <v>45635</v>
+      <c r="J37" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K37" t="n">
         <v>487000</v>
@@ -2120,15 +1989,7 @@
       <c r="L37" t="n">
         <v>27569070</v>
       </c>
-      <c r="M37" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N37" s="2" t="n">
-        <v>485000</v>
-      </c>
-      <c r="O37" t="n">
-        <v>27455850</v>
-      </c>
+      <c r="M37" s="2" t="n"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2156,7 +2017,7 @@
           <t xml:space="preserve">6 </t>
         </is>
       </c>
-      <c r="G38" s="1" t="n">
+      <c r="G38" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H38" t="n">
@@ -2165,24 +2026,8 @@
       <c r="I38" t="n">
         <v>28021400</v>
       </c>
-      <c r="J38" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="K38" t="n">
-        <v>470000</v>
-      </c>
-      <c r="L38" t="n">
-        <v>28021400</v>
-      </c>
-      <c r="M38" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N38" s="3" t="n">
-        <v>475000</v>
-      </c>
-      <c r="O38" t="n">
-        <v>28319500</v>
-      </c>
+      <c r="J38" s="2" t="n"/>
+      <c r="M38" s="2" t="n"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2210,7 +2055,7 @@
           <t xml:space="preserve">5 </t>
         </is>
       </c>
-      <c r="G39" s="1" t="n">
+      <c r="G39" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H39" t="n">
@@ -2219,8 +2064,8 @@
       <c r="I39" t="n">
         <v>28973100</v>
       </c>
-      <c r="J39" s="1" t="n">
-        <v>45635</v>
+      <c r="J39" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K39" t="n">
         <v>442000</v>
@@ -2228,15 +2073,7 @@
       <c r="L39" t="n">
         <v>28973100</v>
       </c>
-      <c r="M39" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N39" t="n">
-        <v>442000</v>
-      </c>
-      <c r="O39" t="n">
-        <v>28973100</v>
-      </c>
+      <c r="M39" s="2" t="n"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2264,7 +2101,7 @@
           <t xml:space="preserve">5 </t>
         </is>
       </c>
-      <c r="G40" s="1" t="n">
+      <c r="G40" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H40" t="n">
@@ -2273,8 +2110,8 @@
       <c r="I40" t="n">
         <v>28973100</v>
       </c>
-      <c r="J40" s="1" t="n">
-        <v>45635</v>
+      <c r="J40" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K40" t="n">
         <v>442000</v>
@@ -2282,15 +2119,7 @@
       <c r="L40" t="n">
         <v>28973100</v>
       </c>
-      <c r="M40" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N40" t="n">
-        <v>442000</v>
-      </c>
-      <c r="O40" t="n">
-        <v>28973100</v>
-      </c>
+      <c r="M40" s="2" t="n"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2318,7 +2147,7 @@
           <t xml:space="preserve">4 </t>
         </is>
       </c>
-      <c r="G41" s="1" t="n">
+      <c r="G41" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H41" t="n">
@@ -2327,8 +2156,8 @@
       <c r="I41" t="n">
         <v>29124700</v>
       </c>
-      <c r="J41" s="1" t="n">
-        <v>45635</v>
+      <c r="J41" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K41" t="n">
         <v>415000</v>
@@ -2336,15 +2165,7 @@
       <c r="L41" t="n">
         <v>29124700</v>
       </c>
-      <c r="M41" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N41" t="n">
-        <v>415000</v>
-      </c>
-      <c r="O41" t="n">
-        <v>29124700</v>
-      </c>
+      <c r="M41" s="2" t="n"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2372,7 +2193,7 @@
           <t xml:space="preserve">3 </t>
         </is>
       </c>
-      <c r="G42" s="1" t="n">
+      <c r="G42" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H42" t="n">
@@ -2381,24 +2202,8 @@
       <c r="I42" t="n">
         <v>29174880</v>
       </c>
-      <c r="J42" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="K42" t="n">
-        <v>456000</v>
-      </c>
-      <c r="L42" t="n">
-        <v>29174880</v>
-      </c>
-      <c r="M42" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N42" t="n">
-        <v>456000</v>
-      </c>
-      <c r="O42" t="n">
-        <v>29174880</v>
-      </c>
+      <c r="J42" s="2" t="n"/>
+      <c r="M42" s="2" t="n"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2426,7 +2231,7 @@
           <t xml:space="preserve">5 </t>
         </is>
       </c>
-      <c r="G43" s="1" t="n">
+      <c r="G43" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H43" t="n">
@@ -2435,8 +2240,8 @@
       <c r="I43" t="n">
         <v>29334800</v>
       </c>
-      <c r="J43" s="1" t="n">
-        <v>45635</v>
+      <c r="J43" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K43" t="n">
         <v>440000</v>
@@ -2444,15 +2249,7 @@
       <c r="L43" t="n">
         <v>29334800</v>
       </c>
-      <c r="M43" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N43" t="n">
-        <v>440000</v>
-      </c>
-      <c r="O43" t="n">
-        <v>29334800</v>
-      </c>
+      <c r="M43" s="2" t="n"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2480,7 +2277,7 @@
           <t xml:space="preserve">3 </t>
         </is>
       </c>
-      <c r="G44" s="1" t="n">
+      <c r="G44" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H44" t="n">
@@ -2489,8 +2286,8 @@
       <c r="I44" t="n">
         <v>29366820</v>
       </c>
-      <c r="J44" s="1" t="n">
-        <v>45635</v>
+      <c r="J44" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K44" t="n">
         <v>459000</v>
@@ -2498,15 +2295,7 @@
       <c r="L44" t="n">
         <v>29366820</v>
       </c>
-      <c r="M44" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N44" t="n">
-        <v>459000</v>
-      </c>
-      <c r="O44" t="n">
-        <v>29366820</v>
-      </c>
+      <c r="M44" s="2" t="n"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2534,7 +2323,7 @@
           <t xml:space="preserve">3 </t>
         </is>
       </c>
-      <c r="G45" s="1" t="n">
+      <c r="G45" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H45" t="n">
@@ -2543,8 +2332,8 @@
       <c r="I45" t="n">
         <v>29472940</v>
       </c>
-      <c r="J45" s="1" t="n">
-        <v>45635</v>
+      <c r="J45" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K45" t="n">
         <v>434000</v>
@@ -2552,15 +2341,7 @@
       <c r="L45" t="n">
         <v>29472940</v>
       </c>
-      <c r="M45" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N45" t="n">
-        <v>434000</v>
-      </c>
-      <c r="O45" t="n">
-        <v>29472940</v>
-      </c>
+      <c r="M45" s="2" t="n"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2588,7 +2369,7 @@
           <t xml:space="preserve">7 </t>
         </is>
       </c>
-      <c r="G46" s="1" t="n">
+      <c r="G46" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H46" t="n">
@@ -2597,24 +2378,8 @@
       <c r="I46" t="n">
         <v>29968950</v>
       </c>
-      <c r="J46" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="K46" t="n">
-        <v>443000</v>
-      </c>
-      <c r="L46" t="n">
-        <v>29968950</v>
-      </c>
-      <c r="M46" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N46" t="n">
-        <v>443000</v>
-      </c>
-      <c r="O46" t="n">
-        <v>29968950</v>
-      </c>
+      <c r="J46" s="2" t="n"/>
+      <c r="M46" s="2" t="n"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2642,7 +2407,7 @@
           <t xml:space="preserve">6 </t>
         </is>
       </c>
-      <c r="G47" s="1" t="n">
+      <c r="G47" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H47" t="n">
@@ -2651,8 +2416,8 @@
       <c r="I47" t="n">
         <v>30132860</v>
       </c>
-      <c r="J47" s="1" t="n">
-        <v>45635</v>
+      <c r="J47" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K47" t="n">
         <v>443000</v>
@@ -2660,15 +2425,7 @@
       <c r="L47" t="n">
         <v>30132860</v>
       </c>
-      <c r="M47" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N47" t="n">
-        <v>443000</v>
-      </c>
-      <c r="O47" t="n">
-        <v>30132860</v>
-      </c>
+      <c r="M47" s="2" t="n"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2696,7 +2453,7 @@
           <t xml:space="preserve">6 </t>
         </is>
       </c>
-      <c r="G48" s="1" t="n">
+      <c r="G48" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H48" t="n">
@@ -2705,8 +2462,8 @@
       <c r="I48" t="n">
         <v>30132860</v>
       </c>
-      <c r="J48" s="1" t="n">
-        <v>45635</v>
+      <c r="J48" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K48" t="n">
         <v>443000</v>
@@ -2714,15 +2471,7 @@
       <c r="L48" t="n">
         <v>30132860</v>
       </c>
-      <c r="M48" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N48" t="n">
-        <v>443000</v>
-      </c>
-      <c r="O48" t="n">
-        <v>30132860</v>
-      </c>
+      <c r="M48" s="2" t="n"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2750,7 +2499,7 @@
           <t xml:space="preserve">6 </t>
         </is>
       </c>
-      <c r="G49" s="1" t="n">
+      <c r="G49" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H49" t="n">
@@ -2759,8 +2508,8 @@
       <c r="I49" t="n">
         <v>30132860</v>
       </c>
-      <c r="J49" s="1" t="n">
-        <v>45635</v>
+      <c r="J49" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K49" t="n">
         <v>443000</v>
@@ -2795,7 +2544,7 @@
           <t xml:space="preserve">2 </t>
         </is>
       </c>
-      <c r="G50" s="1" t="n">
+      <c r="G50" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H50" t="n">
@@ -2804,8 +2553,8 @@
       <c r="I50" t="n">
         <v>30371700</v>
       </c>
-      <c r="J50" s="1" t="n">
-        <v>45635</v>
+      <c r="J50" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K50" t="n">
         <v>435000</v>
@@ -2840,7 +2589,7 @@
           <t xml:space="preserve">2 </t>
         </is>
       </c>
-      <c r="G51" s="1" t="n">
+      <c r="G51" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H51" t="n">
@@ -2849,8 +2598,8 @@
       <c r="I51" t="n">
         <v>30371700</v>
       </c>
-      <c r="J51" s="1" t="n">
-        <v>45635</v>
+      <c r="J51" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K51" t="n">
         <v>435000</v>
@@ -2885,7 +2634,7 @@
           <t xml:space="preserve">2 </t>
         </is>
       </c>
-      <c r="G52" s="1" t="n">
+      <c r="G52" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H52" t="n">
@@ -2894,24 +2643,8 @@
       <c r="I52" t="n">
         <v>30371700</v>
       </c>
-      <c r="J52" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="K52" t="n">
-        <v>435000</v>
-      </c>
-      <c r="L52" t="n">
-        <v>30371700</v>
-      </c>
-      <c r="M52" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N52" t="n">
-        <v>435000</v>
-      </c>
-      <c r="O52" t="n">
-        <v>30371700</v>
-      </c>
+      <c r="J52" s="2" t="n"/>
+      <c r="M52" s="2" t="n"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2939,7 +2672,7 @@
           <t xml:space="preserve">6 </t>
         </is>
       </c>
-      <c r="G53" s="1" t="n">
+      <c r="G53" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H53" t="n">
@@ -2948,8 +2681,8 @@
       <c r="I53" t="n">
         <v>30547760</v>
       </c>
-      <c r="J53" s="1" t="n">
-        <v>45635</v>
+      <c r="J53" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K53" t="n">
         <v>421000</v>
@@ -2957,15 +2690,7 @@
       <c r="L53" t="n">
         <v>30547760</v>
       </c>
-      <c r="M53" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N53" t="n">
-        <v>421000</v>
-      </c>
-      <c r="O53" t="n">
-        <v>30547760</v>
-      </c>
+      <c r="M53" s="2" t="n"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2993,7 +2718,7 @@
           <t xml:space="preserve">2 </t>
         </is>
       </c>
-      <c r="G54" s="1" t="n">
+      <c r="G54" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H54" t="n">
@@ -3002,8 +2727,8 @@
       <c r="I54" t="n">
         <v>30665060</v>
       </c>
-      <c r="J54" s="1" t="n">
-        <v>45635</v>
+      <c r="J54" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K54" t="n">
         <v>433000</v>
@@ -3011,15 +2736,7 @@
       <c r="L54" t="n">
         <v>30665060</v>
       </c>
-      <c r="M54" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N54" t="n">
-        <v>433000</v>
-      </c>
-      <c r="O54" t="n">
-        <v>30665060</v>
-      </c>
+      <c r="M54" s="2" t="n"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3047,7 +2764,7 @@
           <t xml:space="preserve">4 </t>
         </is>
       </c>
-      <c r="G55" s="1" t="n">
+      <c r="G55" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H55" t="n">
@@ -3056,8 +2773,8 @@
       <c r="I55" t="n">
         <v>30809020</v>
       </c>
-      <c r="J55" s="1" t="n">
-        <v>45635</v>
+      <c r="J55" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K55" t="n">
         <v>439000</v>
@@ -3065,15 +2782,7 @@
       <c r="L55" t="n">
         <v>30809020</v>
       </c>
-      <c r="M55" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N55" t="n">
-        <v>439000</v>
-      </c>
-      <c r="O55" t="n">
-        <v>30809020</v>
-      </c>
+      <c r="M55" s="2" t="n"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3101,7 +2810,7 @@
           <t xml:space="preserve">4 </t>
         </is>
       </c>
-      <c r="G56" s="1" t="n">
+      <c r="G56" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H56" t="n">
@@ -3110,8 +2819,8 @@
       <c r="I56" t="n">
         <v>30864240</v>
       </c>
-      <c r="J56" s="1" t="n">
-        <v>45635</v>
+      <c r="J56" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K56" t="n">
         <v>433000</v>
@@ -3119,15 +2828,7 @@
       <c r="L56" t="n">
         <v>30864240</v>
       </c>
-      <c r="M56" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N56" t="n">
-        <v>433000</v>
-      </c>
-      <c r="O56" t="n">
-        <v>30864240</v>
-      </c>
+      <c r="M56" s="2" t="n"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3155,7 +2856,7 @@
           <t xml:space="preserve">6 </t>
         </is>
       </c>
-      <c r="G57" s="1" t="n">
+      <c r="G57" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H57" t="n">
@@ -3164,8 +2865,8 @@
       <c r="I57" t="n">
         <v>30892050</v>
       </c>
-      <c r="J57" s="1" t="n">
-        <v>45635</v>
+      <c r="J57" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K57" t="n">
         <v>441000</v>
@@ -3173,15 +2874,7 @@
       <c r="L57" t="n">
         <v>30892050</v>
       </c>
-      <c r="M57" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N57" t="n">
-        <v>441000</v>
-      </c>
-      <c r="O57" t="n">
-        <v>30892050</v>
-      </c>
+      <c r="M57" s="2" t="n"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3209,7 +2902,7 @@
           <t xml:space="preserve">4 </t>
         </is>
       </c>
-      <c r="G58" s="1" t="n">
+      <c r="G58" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H58" t="n">
@@ -3218,8 +2911,8 @@
       <c r="I58" t="n">
         <v>31149360</v>
       </c>
-      <c r="J58" s="1" t="n">
-        <v>45635</v>
+      <c r="J58" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K58" t="n">
         <v>437000</v>
@@ -3227,15 +2920,7 @@
       <c r="L58" t="n">
         <v>31149360</v>
       </c>
-      <c r="M58" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N58" t="n">
-        <v>437000</v>
-      </c>
-      <c r="O58" t="n">
-        <v>31149360</v>
-      </c>
+      <c r="M58" s="2" t="n"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3263,7 +2948,7 @@
           <t xml:space="preserve">5 </t>
         </is>
       </c>
-      <c r="G59" s="1" t="n">
+      <c r="G59" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H59" t="n">
@@ -3272,8 +2957,8 @@
       <c r="I59" t="n">
         <v>35934800</v>
       </c>
-      <c r="J59" s="1" t="n">
-        <v>45635</v>
+      <c r="J59" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K59" t="n">
         <v>440000</v>
@@ -3281,15 +2966,7 @@
       <c r="L59" t="n">
         <v>35934800</v>
       </c>
-      <c r="M59" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N59" t="n">
-        <v>440000</v>
-      </c>
-      <c r="O59" t="n">
-        <v>35934800</v>
-      </c>
+      <c r="M59" s="2" t="n"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3317,7 +2994,7 @@
           <t xml:space="preserve">5 </t>
         </is>
       </c>
-      <c r="G60" s="1" t="n">
+      <c r="G60" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H60" t="n">
@@ -3326,8 +3003,8 @@
       <c r="I60" t="n">
         <v>36428460</v>
       </c>
-      <c r="J60" s="1" t="n">
-        <v>45635</v>
+      <c r="J60" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K60" t="n">
         <v>438000</v>
@@ -3335,15 +3012,7 @@
       <c r="L60" t="n">
         <v>36428460</v>
       </c>
-      <c r="M60" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N60" t="n">
-        <v>438000</v>
-      </c>
-      <c r="O60" t="n">
-        <v>36428460</v>
-      </c>
+      <c r="M60" s="2" t="n"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3371,7 +3040,7 @@
           <t xml:space="preserve">7 </t>
         </is>
       </c>
-      <c r="G61" s="1" t="n">
+      <c r="G61" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H61" t="n">
@@ -3380,24 +3049,8 @@
       <c r="I61" t="n">
         <v>39214450</v>
       </c>
-      <c r="J61" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="K61" t="n">
-        <v>407000</v>
-      </c>
-      <c r="L61" t="n">
-        <v>39214450</v>
-      </c>
-      <c r="M61" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N61" t="n">
-        <v>407000</v>
-      </c>
-      <c r="O61" t="n">
-        <v>39214450</v>
-      </c>
+      <c r="J61" s="2" t="n"/>
+      <c r="M61" s="2" t="n"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3425,7 +3078,7 @@
           <t xml:space="preserve">6 </t>
         </is>
       </c>
-      <c r="G62" s="1" t="n">
+      <c r="G62" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H62" t="n">
@@ -3434,8 +3087,8 @@
       <c r="I62" t="n">
         <v>39798820</v>
       </c>
-      <c r="J62" s="1" t="n">
-        <v>45635</v>
+      <c r="J62" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K62" t="n">
         <v>422000</v>
@@ -3443,15 +3096,7 @@
       <c r="L62" t="n">
         <v>39798820</v>
       </c>
-      <c r="M62" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N62" t="n">
-        <v>422000</v>
-      </c>
-      <c r="O62" t="n">
-        <v>39798820</v>
-      </c>
+      <c r="M62" s="2" t="n"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3479,7 +3124,7 @@
           <t xml:space="preserve">6 </t>
         </is>
       </c>
-      <c r="G63" s="1" t="n">
+      <c r="G63" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H63" t="n">
@@ -3488,24 +3133,8 @@
       <c r="I63" t="n">
         <v>39865280</v>
       </c>
-      <c r="J63" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="K63" t="n">
-        <v>416000</v>
-      </c>
-      <c r="L63" t="n">
-        <v>39865280</v>
-      </c>
-      <c r="M63" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N63" t="n">
-        <v>416000</v>
-      </c>
-      <c r="O63" t="n">
-        <v>39865280</v>
-      </c>
+      <c r="J63" s="2" t="n"/>
+      <c r="M63" s="2" t="n"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3533,7 +3162,7 @@
           <t xml:space="preserve">7 </t>
         </is>
       </c>
-      <c r="G64" s="1" t="n">
+      <c r="G64" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H64" t="n">
@@ -3542,8 +3171,8 @@
       <c r="I64" t="n">
         <v>40431150</v>
       </c>
-      <c r="J64" s="1" t="n">
-        <v>45635</v>
+      <c r="J64" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K64" t="n">
         <v>405000</v>
@@ -3551,15 +3180,7 @@
       <c r="L64" t="n">
         <v>40431150</v>
       </c>
-      <c r="M64" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N64" t="n">
-        <v>405000</v>
-      </c>
-      <c r="O64" t="n">
-        <v>40431150</v>
-      </c>
+      <c r="M64" s="2" t="n"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3587,7 +3208,7 @@
           <t xml:space="preserve">6 </t>
         </is>
       </c>
-      <c r="G65" s="1" t="n">
+      <c r="G65" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H65" t="n">
@@ -3596,8 +3217,8 @@
       <c r="I65" t="n">
         <v>40625940</v>
       </c>
-      <c r="J65" s="1" t="n">
-        <v>45635</v>
+      <c r="J65" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K65" t="n">
         <v>422000</v>
@@ -3605,15 +3226,7 @@
       <c r="L65" t="n">
         <v>40625940</v>
       </c>
-      <c r="M65" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N65" t="n">
-        <v>422000</v>
-      </c>
-      <c r="O65" t="n">
-        <v>40625940</v>
-      </c>
+      <c r="M65" s="2" t="n"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3641,7 +3254,7 @@
           <t xml:space="preserve">6 </t>
         </is>
       </c>
-      <c r="G66" s="1" t="n">
+      <c r="G66" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H66" t="n">
@@ -3650,8 +3263,8 @@
       <c r="I66" t="n">
         <v>40625940</v>
       </c>
-      <c r="J66" s="1" t="n">
-        <v>45635</v>
+      <c r="J66" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K66" t="n">
         <v>422000</v>
@@ -3659,15 +3272,7 @@
       <c r="L66" t="n">
         <v>40625940</v>
       </c>
-      <c r="M66" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N66" t="n">
-        <v>422000</v>
-      </c>
-      <c r="O66" t="n">
-        <v>40625940</v>
-      </c>
+      <c r="M66" s="2" t="n"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3695,7 +3300,7 @@
           <t xml:space="preserve">6 </t>
         </is>
       </c>
-      <c r="G67" s="1" t="n">
+      <c r="G67" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H67" t="n">
@@ -3704,8 +3309,8 @@
       <c r="I67" t="n">
         <v>40697280</v>
       </c>
-      <c r="J67" s="1" t="n">
-        <v>45635</v>
+      <c r="J67" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K67" t="n">
         <v>416000</v>
@@ -3713,15 +3318,7 @@
       <c r="L67" t="n">
         <v>40697280</v>
       </c>
-      <c r="M67" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N67" t="n">
-        <v>416000</v>
-      </c>
-      <c r="O67" t="n">
-        <v>40697280</v>
-      </c>
+      <c r="M67" s="2" t="n"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3749,7 +3346,7 @@
           <t xml:space="preserve">2 </t>
         </is>
       </c>
-      <c r="G68" s="1" t="n">
+      <c r="G68" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H68" t="n">
@@ -3758,8 +3355,8 @@
       <c r="I68" t="n">
         <v>41669550</v>
       </c>
-      <c r="J68" s="1" t="n">
-        <v>45635</v>
+      <c r="J68" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K68" t="n">
         <v>419000</v>
@@ -3767,15 +3364,7 @@
       <c r="L68" t="n">
         <v>41669550</v>
       </c>
-      <c r="M68" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N68" t="n">
-        <v>419000</v>
-      </c>
-      <c r="O68" t="n">
-        <v>41669550</v>
-      </c>
+      <c r="M68" s="2" t="n"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3803,7 +3392,7 @@
           <t xml:space="preserve">2 </t>
         </is>
       </c>
-      <c r="G69" s="1" t="n">
+      <c r="G69" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H69" t="n">
@@ -3812,24 +3401,8 @@
       <c r="I69" t="n">
         <v>41669550</v>
       </c>
-      <c r="J69" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="K69" t="n">
-        <v>419000</v>
-      </c>
-      <c r="L69" t="n">
-        <v>41669550</v>
-      </c>
-      <c r="M69" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N69" t="n">
-        <v>419000</v>
-      </c>
-      <c r="O69" t="n">
-        <v>41669550</v>
-      </c>
+      <c r="J69" s="2" t="n"/>
+      <c r="M69" s="2" t="n"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3857,7 +3430,7 @@
           <t xml:space="preserve">2 </t>
         </is>
       </c>
-      <c r="G70" s="1" t="n">
+      <c r="G70" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H70" t="n">
@@ -3866,24 +3439,8 @@
       <c r="I70" t="n">
         <v>41669550</v>
       </c>
-      <c r="J70" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="K70" t="n">
-        <v>419000</v>
-      </c>
-      <c r="L70" t="n">
-        <v>41669550</v>
-      </c>
-      <c r="M70" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N70" t="n">
-        <v>419000</v>
-      </c>
-      <c r="O70" t="n">
-        <v>41669550</v>
-      </c>
+      <c r="J70" s="2" t="n"/>
+      <c r="M70" s="2" t="n"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3911,7 +3468,7 @@
           <t xml:space="preserve">2 </t>
         </is>
       </c>
-      <c r="G71" s="1" t="n">
+      <c r="G71" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H71" t="n">
@@ -3920,8 +3477,8 @@
       <c r="I71" t="n">
         <v>41679960</v>
       </c>
-      <c r="J71" s="1" t="n">
-        <v>45635</v>
+      <c r="J71" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K71" t="n">
         <v>413000</v>
@@ -3929,15 +3486,7 @@
       <c r="L71" t="n">
         <v>41679960</v>
       </c>
-      <c r="M71" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N71" t="n">
-        <v>413000</v>
-      </c>
-      <c r="O71" t="n">
-        <v>41679960</v>
-      </c>
+      <c r="M71" s="2" t="n"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3965,7 +3514,7 @@
           <t xml:space="preserve">6 </t>
         </is>
       </c>
-      <c r="G72" s="1" t="n">
+      <c r="G72" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="H72" t="n">
@@ -3974,8 +3523,8 @@
       <c r="I72" t="n">
         <v>42452690</v>
       </c>
-      <c r="J72" s="1" t="n">
-        <v>45635</v>
+      <c r="J72" s="2" t="n">
+        <v>45648</v>
       </c>
       <c r="K72" t="n">
         <v>443000</v>
@@ -3983,14 +3532,762 @@
       <c r="L72" t="n">
         <v>42452690</v>
       </c>
-      <c r="M72" s="1" t="n">
-        <v>45635</v>
-      </c>
-      <c r="N72" t="n">
-        <v>443000</v>
-      </c>
-      <c r="O72" t="n">
-        <v>42452690</v>
+      <c r="M72" s="2" t="n"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>35.58</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">8  </t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2 </t>
+        </is>
+      </c>
+      <c r="G73" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H73" t="n">
+        <v>535000</v>
+      </c>
+      <c r="I73" t="n">
+        <v>19035300</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>163</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>35.62</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6  </t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 </t>
+        </is>
+      </c>
+      <c r="G74" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H74" t="n">
+        <v>535000</v>
+      </c>
+      <c r="I74" t="n">
+        <v>19056700</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>35.62</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4  </t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 </t>
+        </is>
+      </c>
+      <c r="G75" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H75" t="n">
+        <v>535000</v>
+      </c>
+      <c r="I75" t="n">
+        <v>19056700</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>145</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>35.62</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3  </t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 </t>
+        </is>
+      </c>
+      <c r="G76" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H76" t="n">
+        <v>535000</v>
+      </c>
+      <c r="I76" t="n">
+        <v>19056700</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>36.52</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4  </t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5 </t>
+        </is>
+      </c>
+      <c r="G77" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H77" t="n">
+        <v>530000</v>
+      </c>
+      <c r="I77" t="n">
+        <v>19355600</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>194</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>36.52</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3  </t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5 </t>
+        </is>
+      </c>
+      <c r="G78" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H78" t="n">
+        <v>530000</v>
+      </c>
+      <c r="I78" t="n">
+        <v>19355600</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>108</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>36.52</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5  </t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 </t>
+        </is>
+      </c>
+      <c r="G79" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H79" t="n">
+        <v>530000</v>
+      </c>
+      <c r="I79" t="n">
+        <v>19355600</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>36.52</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3  </t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 </t>
+        </is>
+      </c>
+      <c r="G80" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H80" t="n">
+        <v>530000</v>
+      </c>
+      <c r="I80" t="n">
+        <v>19355600</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>299</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>36.82</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6  </t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7 </t>
+        </is>
+      </c>
+      <c r="G81" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H81" t="n">
+        <v>530000</v>
+      </c>
+      <c r="I81" t="n">
+        <v>19514600</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>293</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>36.82</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5  </t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7 </t>
+        </is>
+      </c>
+      <c r="G82" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H82" t="n">
+        <v>530000</v>
+      </c>
+      <c r="I82" t="n">
+        <v>19514600</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>287</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>36.82</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4  </t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7 </t>
+        </is>
+      </c>
+      <c r="G83" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H83" t="n">
+        <v>530000</v>
+      </c>
+      <c r="I83" t="n">
+        <v>19514600</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>281</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>36.82</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3  </t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7 </t>
+        </is>
+      </c>
+      <c r="G84" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H84" t="n">
+        <v>530000</v>
+      </c>
+      <c r="I84" t="n">
+        <v>19514600</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>44.5</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2  </t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 </t>
+        </is>
+      </c>
+      <c r="G85" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H85" t="n">
+        <v>467000</v>
+      </c>
+      <c r="I85" t="n">
+        <v>20781500</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>40.6</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5  </t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 </t>
+        </is>
+      </c>
+      <c r="G86" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H86" t="n">
+        <v>514000</v>
+      </c>
+      <c r="I86" t="n">
+        <v>20868400</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>227</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>47.36</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">9  </t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5 </t>
+        </is>
+      </c>
+      <c r="G87" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H87" t="n">
+        <v>465000</v>
+      </c>
+      <c r="I87" t="n">
+        <v>22022400</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>56.61</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5  </t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2 </t>
+        </is>
+      </c>
+      <c r="G88" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H88" t="n">
+        <v>487000</v>
+      </c>
+      <c r="I88" t="n">
+        <v>27569070</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>56.61</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4  </t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2 </t>
+        </is>
+      </c>
+      <c r="G89" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H89" t="n">
+        <v>487000</v>
+      </c>
+      <c r="I89" t="n">
+        <v>27569070</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>70.18</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4  </t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 </t>
+        </is>
+      </c>
+      <c r="G90" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H90" t="n">
+        <v>439000</v>
+      </c>
+      <c r="I90" t="n">
+        <v>30809020</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>70.18</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3  </t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 </t>
+        </is>
+      </c>
+      <c r="G91" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H91" t="n">
+        <v>439000</v>
+      </c>
+      <c r="I91" t="n">
+        <v>30809020</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>79.52</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4  </t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 </t>
+        </is>
+      </c>
+      <c r="G92" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H92" t="n">
+        <v>445000</v>
+      </c>
+      <c r="I92" t="n">
+        <v>35386400</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>79.52</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3  </t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 </t>
+        </is>
+      </c>
+      <c r="G93" s="6" t="n">
+        <v>45648</v>
+      </c>
+      <c r="H93" t="n">
+        <v>445000</v>
+      </c>
+      <c r="I93" t="n">
+        <v>35386400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>